<commit_message>
event ID, new logo
</commit_message>
<xml_diff>
--- a/controllers/eventDetails.xlsx
+++ b/controllers/eventDetails.xlsx
@@ -3,18 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="20000" firstSheet="0" activeTab="7"/>
-  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Event Details" state="show" r:id="rId4"/>
+    <sheet sheetId="1" name="August" state="show" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+  <si>
+    <t>Event ID</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
   <si>
     <t>Start Date</t>
   </si>
@@ -22,10 +28,88 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Club Name</t>
-  </si>
-  <si>
-    <t>Event Name</t>
+    <t>Rooms</t>
+  </si>
+  <si>
+    <t>Booked By</t>
+  </si>
+  <si>
+    <t>-LKKaZGZAHjHCwBCkhPW</t>
+  </si>
+  <si>
+    <t>External</t>
+  </si>
+  <si>
+    <t>Web Dev Workshop</t>
+  </si>
+  <si>
+    <t>Tuesday, 21st August 2018</t>
+  </si>
+  <si>
+    <t>Sunday, 26th August 2018</t>
+  </si>
+  <si>
+    <t>AB-5-201, AB-5-202, AB-5-203, AB-5-204</t>
+  </si>
+  <si>
+    <t>Bhawesh Bhansali</t>
+  </si>
+  <si>
+    <t>-LKKe4SAl7bWFfZVPEQz</t>
+  </si>
+  <si>
+    <t>Rotaract Work</t>
+  </si>
+  <si>
+    <t>Thursday, 23rd August 2018</t>
+  </si>
+  <si>
+    <t>NLH-201, NLH-202</t>
+  </si>
+  <si>
+    <t>Daksh</t>
+  </si>
+  <si>
+    <t>dummcook46891</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>Cooking</t>
+  </si>
+  <si>
+    <t>AB-5-310, AB-5-311</t>
+  </si>
+  <si>
+    <t>Bhawesh</t>
+  </si>
+  <si>
+    <t>dummlits594030</t>
+  </si>
+  <si>
+    <t>litstock</t>
+  </si>
+  <si>
+    <t>Saturday, 25th August 2018</t>
+  </si>
+  <si>
+    <t>NLH-303, NLH-305</t>
+  </si>
+  <si>
+    <t>vibhuti</t>
+  </si>
+  <si>
+    <t>dummplan848023</t>
+  </si>
+  <si>
+    <t>Planning Workshop</t>
+  </si>
+  <si>
+    <t>Friday, 24th August 2018</t>
+  </si>
+  <si>
+    <t>AB-5-201, AB-5-202</t>
   </si>
 </sst>
 </file>
@@ -402,14 +486,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="2" width="30" customWidth="1"/>
-    <col min="3" max="4" width="40" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,6 +507,130 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>